<commit_message>
final becuse rebase failed
</commit_message>
<xml_diff>
--- a/HW03/nondense.xlsx
+++ b/HW03/nondense.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\collage\Data Structure\DSA\HW03\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14AF4ED5-4757-4E10-BE2C-747B827345E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
-    <sheet name="nondense" sheetId="1" r:id="rId1"/>
+    <sheet name="f" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>m</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -29,35 +30,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t1</t>
+    <t>n^2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>t3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>t4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>t5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>m*n</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>average t</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>m*n^2</t>
+    <t>t</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -135,7 +112,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C5700"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -587,7 +564,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,7 +576,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -611,7 +588,7 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -623,7 +600,7 @@
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -635,7 +612,7 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -647,7 +624,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -748,13 +725,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-TW"/>
-              <a:t>O(mn)</a:t>
+              <a:t>nondense with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+              <a:t> O(n)</a:t>
             </a:r>
             <a:endParaRPr lang="zh-TW" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -819,294 +799,294 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>nondense!$J$2:$J$47</c:f>
+              <c:f>f!$B$2:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>110000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>130000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>140000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>150000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>170000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>190000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>200000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>300000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>400000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1100000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1200000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1300000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1400000</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1600000</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1700000</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1800000</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1900000</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>7000000</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>10000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>nondense!$L$2:$L$47</c:f>
+              <c:f>f!$D$2:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>2.9599999999999998E-2</c:v>
+                  <c:v>1E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5600000000000001E-2</c:v>
+                  <c:v>1.0319999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12079999999999999</c:v>
+                  <c:v>3.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17859999999999995</c:v>
+                  <c:v>6.7600000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20940000000000003</c:v>
+                  <c:v>1.3010000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24679999999999999</c:v>
+                  <c:v>2.2620000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.28759999999999997</c:v>
+                  <c:v>3.3355000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35299999999999998</c:v>
+                  <c:v>4.4448000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40920000000000006</c:v>
+                  <c:v>5.9390999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44359999999999999</c:v>
+                  <c:v>7.9140000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.50940000000000007</c:v>
+                  <c:v>9.8571000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.54060000000000008</c:v>
+                  <c:v>0.11988</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.63119999999999998</c:v>
+                  <c:v>0.143481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.66220000000000001</c:v>
+                  <c:v>0.16892399999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.7</c:v>
+                  <c:v>0.201735</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.7278</c:v>
+                  <c:v>0.240096</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.80280000000000007</c:v>
+                  <c:v>0.27160899999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.82159999999999989</c:v>
+                  <c:v>0.31307400000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.90860000000000007</c:v>
+                  <c:v>0.367726</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.90600000000000003</c:v>
+                  <c:v>0.38363999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.4498000000000002</c:v>
+                  <c:v>1.00518</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9275999999999995</c:v>
+                  <c:v>1.76868</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4241999999999999</c:v>
+                  <c:v>2.8647499999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.9165999999999999</c:v>
+                  <c:v>4.3067399999999996</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.343</c:v>
+                  <c:v>5.8305800000000003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.9519999999999995</c:v>
+                  <c:v>7.9265600000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.399</c:v>
+                  <c:v>10.345230000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.9863999999999997</c:v>
+                  <c:v>12.7727</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.3298000000000005</c:v>
+                  <c:v>15.828340000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.9779999999999998</c:v>
+                  <c:v>18.397200000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.3986000000000001</c:v>
+                  <c:v>21.9024</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.1457999999999995</c:v>
+                  <c:v>24.91104</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.5004000000000008</c:v>
+                  <c:v>27.966149999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.7573999999999996</c:v>
+                  <c:v>33.766719999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.2138000000000009</c:v>
+                  <c:v>38.538490000000003</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.7356000000000016</c:v>
+                  <c:v>41.8536</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.4134000000000011</c:v>
+                  <c:v>45.10904</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10.047599999999999</c:v>
+                  <c:v>53.365600000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>14.9184</c:v>
+                  <c:v>121.41240000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>19.549199999999999</c:v>
+                  <c:v>219.8108</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>24.788</c:v>
+                  <c:v>317.99650000000003</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>31.042200000000001</c:v>
+                  <c:v>485.31779999999998</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>34.557000000000002</c:v>
+                  <c:v>624.43849999999998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>38.805399999999999</c:v>
+                  <c:v>800.80799999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>45.347999999999999</c:v>
+                  <c:v>1085.076</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>49.859000000000002</c:v>
+                  <c:v>1289.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1114,7 +1094,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FDFA-4035-BF37-00FA06EF5329}"/>
+              <c16:uniqueId val="{00000000-1383-4DD0-A18C-DD0BC4EFFA9D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1126,11 +1106,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="781601039"/>
-        <c:axId val="781601455"/>
+        <c:axId val="600399936"/>
+        <c:axId val="600399280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="781601039"/>
+        <c:axId val="600399936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1150,6 +1130,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1187,12 +1222,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="781601455"/>
+        <c:crossAx val="600399280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="781601455"/>
+        <c:axId val="600399280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1212,6 +1247,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>time (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1249,7 +1340,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="781601039"/>
+        <c:crossAx val="600399936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1263,6 +1354,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1333,13 +1431,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-TW"/>
-              <a:t>O(m*n^2)</a:t>
+              <a:t>nondense wit O(n^2)</a:t>
             </a:r>
             <a:endParaRPr lang="zh-TW" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1404,294 +1501,294 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>nondense!$K$2:$K$47</c:f>
+              <c:f>f!$C$2:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>100000</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>400000</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>900000</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1600000</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2500000</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3600000</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4900000</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6400000</c:v>
+                  <c:v>6400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8100000</c:v>
+                  <c:v>8100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12100000</c:v>
+                  <c:v>12100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14400000</c:v>
+                  <c:v>14400</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16900000</c:v>
+                  <c:v>16900</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19600000</c:v>
+                  <c:v>19600</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22500000</c:v>
+                  <c:v>22500</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25600000</c:v>
+                  <c:v>25600</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28900000</c:v>
+                  <c:v>28900</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32400000</c:v>
+                  <c:v>32400</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36100000</c:v>
+                  <c:v>36100</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40000000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>90000000</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>160000000</c:v>
+                  <c:v>160000</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>250000000</c:v>
+                  <c:v>250000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>360000000</c:v>
+                  <c:v>360000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>490000000</c:v>
+                  <c:v>490000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>640000000</c:v>
+                  <c:v>640000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>810000000</c:v>
+                  <c:v>810000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1000000000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1210000000</c:v>
+                  <c:v>1210000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1440000000</c:v>
+                  <c:v>1440000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1690000000</c:v>
+                  <c:v>1690000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1960000000</c:v>
+                  <c:v>1960000</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2250000000</c:v>
+                  <c:v>2250000</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2560000000</c:v>
+                  <c:v>2560000</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2890000000</c:v>
+                  <c:v>2890000</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3240000000</c:v>
+                  <c:v>3240000</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3610000000</c:v>
+                  <c:v>3610000</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4000000000</c:v>
+                  <c:v>4000000</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9000000000</c:v>
+                  <c:v>9000000</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>16000000000</c:v>
+                  <c:v>16000000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>25000000000</c:v>
+                  <c:v>25000000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>36000000000</c:v>
+                  <c:v>36000000</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>49000000000</c:v>
+                  <c:v>49000000</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>64000000000</c:v>
+                  <c:v>64000000</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>81000000000</c:v>
+                  <c:v>81000000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>100000000000</c:v>
+                  <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>nondense!$L$2:$L$47</c:f>
+              <c:f>f!$D$2:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>2.9599999999999998E-2</c:v>
+                  <c:v>1E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5600000000000001E-2</c:v>
+                  <c:v>1.0319999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12079999999999999</c:v>
+                  <c:v>3.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17859999999999995</c:v>
+                  <c:v>6.7600000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20940000000000003</c:v>
+                  <c:v>1.3010000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24679999999999999</c:v>
+                  <c:v>2.2620000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.28759999999999997</c:v>
+                  <c:v>3.3355000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35299999999999998</c:v>
+                  <c:v>4.4448000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40920000000000006</c:v>
+                  <c:v>5.9390999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44359999999999999</c:v>
+                  <c:v>7.9140000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.50940000000000007</c:v>
+                  <c:v>9.8571000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.54060000000000008</c:v>
+                  <c:v>0.11988</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.63119999999999998</c:v>
+                  <c:v>0.143481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.66220000000000001</c:v>
+                  <c:v>0.16892399999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.7</c:v>
+                  <c:v>0.201735</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.7278</c:v>
+                  <c:v>0.240096</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.80280000000000007</c:v>
+                  <c:v>0.27160899999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.82159999999999989</c:v>
+                  <c:v>0.31307400000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.90860000000000007</c:v>
+                  <c:v>0.367726</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.90600000000000003</c:v>
+                  <c:v>0.38363999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.4498000000000002</c:v>
+                  <c:v>1.00518</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9275999999999995</c:v>
+                  <c:v>1.76868</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4241999999999999</c:v>
+                  <c:v>2.8647499999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.9165999999999999</c:v>
+                  <c:v>4.3067399999999996</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.343</c:v>
+                  <c:v>5.8305800000000003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.9519999999999995</c:v>
+                  <c:v>7.9265600000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.399</c:v>
+                  <c:v>10.345230000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.9863999999999997</c:v>
+                  <c:v>12.7727</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.3298000000000005</c:v>
+                  <c:v>15.828340000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.9779999999999998</c:v>
+                  <c:v>18.397200000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.3986000000000001</c:v>
+                  <c:v>21.9024</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.1457999999999995</c:v>
+                  <c:v>24.91104</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.5004000000000008</c:v>
+                  <c:v>27.966149999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.7573999999999996</c:v>
+                  <c:v>33.766719999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.2138000000000009</c:v>
+                  <c:v>38.538490000000003</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.7356000000000016</c:v>
+                  <c:v>41.8536</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.4134000000000011</c:v>
+                  <c:v>45.10904</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10.047599999999999</c:v>
+                  <c:v>53.365600000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>14.9184</c:v>
+                  <c:v>121.41240000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>19.549199999999999</c:v>
+                  <c:v>219.8108</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>24.788</c:v>
+                  <c:v>317.99650000000003</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>31.042200000000001</c:v>
+                  <c:v>485.31779999999998</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>34.557000000000002</c:v>
+                  <c:v>624.43849999999998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>38.805399999999999</c:v>
+                  <c:v>800.80799999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>45.347999999999999</c:v>
+                  <c:v>1085.076</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>49.859000000000002</c:v>
+                  <c:v>1289.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1699,7 +1796,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FFBA-479B-B1A6-4E24DA680017}"/>
+              <c16:uniqueId val="{00000000-EA22-4F21-8455-F26762D9D0D5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1711,11 +1808,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="871633855"/>
-        <c:axId val="871649247"/>
+        <c:axId val="778171296"/>
+        <c:axId val="778173592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="871633855"/>
+        <c:axId val="778171296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,6 +1832,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>n^2</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1772,12 +1925,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="871649247"/>
+        <c:crossAx val="778173592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="871649247"/>
+        <c:axId val="778173592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1797,6 +1950,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>time (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1834,7 +2043,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="871633855"/>
+        <c:crossAx val="778171296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1848,6 +2057,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2999,20 +3215,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="圖表 1"/>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CEFE9C6-642A-CFE4-4264-B9FD0F62C9DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3029,20 +3251,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>138112</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="圖表 2"/>
+        <xdr:cNvPr id="3" name="圖表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B39490C9-A4FD-B487-55C4-C15DD913658B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3077,7 +3305,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -3089,7 +3317,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -3136,6 +3364,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3171,6 +3416,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3323,1660 +3585,721 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
+      <c r="C2">
+        <f>B2*B2</f>
+        <v>100</v>
+      </c>
       <c r="D2">
-        <v>3.1E-2</v>
-      </c>
-      <c r="E2">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="F2">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="G2">
-        <v>3.1E-2</v>
-      </c>
-      <c r="H2">
-        <v>2.7E-2</v>
-      </c>
-      <c r="J2">
-        <f>A2*B2</f>
-        <v>10000</v>
-      </c>
-      <c r="K2">
-        <f>J2*B2</f>
-        <v>100000</v>
-      </c>
-      <c r="L2">
-        <f>AVERAGE(D2,E2,F2,G2,H2)</f>
-        <v>2.9599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
+      <c r="C3">
+        <f>B3*B3</f>
+        <v>400</v>
+      </c>
       <c r="D3">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="E3">
-        <v>7.8E-2</v>
-      </c>
-      <c r="F3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G3">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="H3">
-        <v>7.8E-2</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J47" si="0">A3*B3</f>
-        <v>20000</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K47" si="1">J3*B3</f>
-        <v>400000</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L47" si="2">AVERAGE(D3,E3,F3,G3,H3)</f>
-        <v>7.5600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.0319999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000</v>
       </c>
       <c r="B4">
         <v>30</v>
       </c>
+      <c r="C4">
+        <f>B4*B4</f>
+        <v>900</v>
+      </c>
       <c r="D4">
-        <v>0.125</v>
-      </c>
-      <c r="E4">
-        <v>0.11</v>
-      </c>
-      <c r="F4">
-        <v>0.13</v>
-      </c>
-      <c r="G4">
-        <v>0.12</v>
-      </c>
-      <c r="H4">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>30000</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>900000</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>0.12079999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.003E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C47" si="0">B5*B5</f>
+        <v>1600</v>
+      </c>
       <c r="D5">
-        <v>0.192</v>
-      </c>
-      <c r="E5">
-        <v>0.159</v>
-      </c>
-      <c r="F5">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="G5">
-        <v>0.188</v>
-      </c>
-      <c r="H5">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="J5">
+        <v>6.7600000000000004E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="D6">
+        <v>1.3010000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1000</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+      <c r="D7">
+        <v>2.2620000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>4900</v>
+      </c>
+      <c r="D8">
+        <v>3.3355000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>6400</v>
+      </c>
+      <c r="D9">
+        <v>4.4448000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1000</v>
+      </c>
+      <c r="B10">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8100</v>
+      </c>
+      <c r="D10">
+        <v>5.9390999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="D11">
+        <v>7.9140000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>12100</v>
+      </c>
+      <c r="D12">
+        <v>9.8571000000000006E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>120</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>14400</v>
+      </c>
+      <c r="D13">
+        <v>0.11988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1000</v>
+      </c>
+      <c r="B14">
+        <v>130</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>16900</v>
+      </c>
+      <c r="D14">
+        <v>0.143481</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1000</v>
+      </c>
+      <c r="B15">
+        <v>140</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>19600</v>
+      </c>
+      <c r="D15">
+        <v>0.16892399999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>22500</v>
+      </c>
+      <c r="D16">
+        <v>0.201735</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1000</v>
+      </c>
+      <c r="B17">
+        <v>160</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>25600</v>
+      </c>
+      <c r="D17">
+        <v>0.240096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1000</v>
+      </c>
+      <c r="B18">
+        <v>170</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>28900</v>
+      </c>
+      <c r="D18">
+        <v>0.27160899999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1000</v>
+      </c>
+      <c r="B19">
+        <v>180</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>32400</v>
+      </c>
+      <c r="D19">
+        <v>0.31307400000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20">
+        <v>190</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>36100</v>
+      </c>
+      <c r="D20">
+        <v>0.367726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="0"/>
         <v>40000</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>1600000</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>0.17859999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1000</v>
-      </c>
-      <c r="B6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>0.219</v>
-      </c>
-      <c r="E6">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="F6">
-        <v>0.218</v>
-      </c>
-      <c r="G6">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="H6">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>50000</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>2500000</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>0.20940000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1000</v>
-      </c>
-      <c r="B7">
-        <v>60</v>
-      </c>
-      <c r="D7">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="E7">
-        <v>0.25</v>
-      </c>
-      <c r="F7">
-        <v>0.25</v>
-      </c>
-      <c r="G7">
-        <v>0.25</v>
-      </c>
-      <c r="H7">
-        <v>0.25</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>60000</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>3600000</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>0.24679999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1000</v>
-      </c>
-      <c r="B8">
-        <v>70</v>
-      </c>
-      <c r="D8">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="E8">
-        <v>0.28100000000000003</v>
-      </c>
-      <c r="F8">
-        <v>0.26600000000000001</v>
-      </c>
-      <c r="G8">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="H8">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>70000</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>4900000</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>0.28759999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1000</v>
-      </c>
-      <c r="B9">
-        <v>80</v>
-      </c>
-      <c r="D9">
-        <v>0.35899999999999999</v>
-      </c>
-      <c r="E9">
-        <v>0.375</v>
-      </c>
-      <c r="F9">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="G9">
-        <v>0.35899999999999999</v>
-      </c>
-      <c r="H9">
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>80000</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>6400000</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0.35299999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1000</v>
-      </c>
-      <c r="B10">
-        <v>90</v>
-      </c>
-      <c r="D10">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="E10">
-        <v>0.42199999999999999</v>
-      </c>
-      <c r="F10">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="G10">
-        <v>0.437</v>
-      </c>
-      <c r="H10">
-        <v>0.375</v>
-      </c>
-      <c r="J10">
+      <c r="D21">
+        <v>0.38363999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1000</v>
+      </c>
+      <c r="B22">
+        <v>300</v>
+      </c>
+      <c r="C22">
         <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>8100000</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>0.40920000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1000</v>
-      </c>
-      <c r="B11">
-        <v>100</v>
-      </c>
-      <c r="D11">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="E11">
-        <v>0.42199999999999999</v>
-      </c>
-      <c r="F11">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="G11">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="H11">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>10000000</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0.44359999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1000</v>
-      </c>
-      <c r="B12">
-        <v>110</v>
-      </c>
-      <c r="D12">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="F12">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="G12">
-        <v>0.5</v>
-      </c>
-      <c r="H12">
-        <v>0.53100000000000003</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>110000</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>12100000</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0.50940000000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1000</v>
-      </c>
-      <c r="B13">
-        <v>120</v>
-      </c>
-      <c r="D13">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="E13">
-        <v>0.5</v>
-      </c>
-      <c r="F13">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="G13">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="H13">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>120000</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>14400000</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
-        <v>0.54060000000000008</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1000</v>
-      </c>
-      <c r="B14">
-        <v>130</v>
-      </c>
-      <c r="D14">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="E14">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="F14">
-        <v>0.64</v>
-      </c>
-      <c r="G14">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="H14">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>130000</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>16900000</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
-        <v>0.63119999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1000</v>
-      </c>
-      <c r="B15">
-        <v>140</v>
-      </c>
-      <c r="D15">
-        <v>0.64</v>
-      </c>
-      <c r="E15">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="F15">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="G15">
-        <v>0.70299999999999996</v>
-      </c>
-      <c r="H15">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>140000</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>19600000</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>0.66220000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1000</v>
-      </c>
-      <c r="B16">
-        <v>150</v>
-      </c>
-      <c r="D16">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="E16">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="F16">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="G16">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="H16">
-        <v>0.75</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>150000</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="1"/>
-        <v>22500000</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1000</v>
-      </c>
-      <c r="B17">
-        <v>160</v>
-      </c>
-      <c r="D17">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="E17">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="F17">
-        <v>0.68700000000000006</v>
-      </c>
-      <c r="G17">
-        <v>0.75</v>
-      </c>
-      <c r="H17">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="J17">
+      <c r="D22">
+        <v>1.00518</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1000</v>
+      </c>
+      <c r="B23">
+        <v>400</v>
+      </c>
+      <c r="C23">
         <f t="shared" si="0"/>
         <v>160000</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>25600000</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>0.7278</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1000</v>
-      </c>
-      <c r="B18">
-        <v>170</v>
-      </c>
-      <c r="D18">
-        <v>0.82799999999999996</v>
-      </c>
-      <c r="E18">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="F18">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="G18">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="H18">
-        <v>0.82799999999999996</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>170000</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>28900000</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>0.80280000000000007</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1000</v>
-      </c>
-      <c r="B19">
-        <v>180</v>
-      </c>
-      <c r="D19">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="E19">
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="F19">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="G19">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="H19">
-        <v>0.874</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>180000</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>32400000</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="2"/>
-        <v>0.82159999999999989</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1000</v>
-      </c>
-      <c r="B20">
-        <v>190</v>
-      </c>
-      <c r="D20">
-        <v>0.86</v>
-      </c>
-      <c r="E20">
-        <v>0.875</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="H20">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>190000</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>36100000</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="2"/>
-        <v>0.90860000000000007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1000</v>
-      </c>
-      <c r="B21">
-        <v>200</v>
-      </c>
-      <c r="D21">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="E21">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="F21">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="G21">
-        <v>0.874</v>
-      </c>
-      <c r="H21">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>200000</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
-        <v>40000000</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>0.90600000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1000</v>
-      </c>
-      <c r="B22">
-        <v>300</v>
-      </c>
-      <c r="D22">
-        <v>1.516</v>
-      </c>
-      <c r="E22">
-        <v>1.4370000000000001</v>
-      </c>
-      <c r="F22">
-        <v>1.421</v>
-      </c>
-      <c r="G22">
-        <v>1.4059999999999999</v>
-      </c>
-      <c r="H22">
-        <v>1.4690000000000001</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="1"/>
-        <v>90000000</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="2"/>
-        <v>1.4498000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1000</v>
-      </c>
-      <c r="B23">
-        <v>400</v>
-      </c>
       <c r="D23">
-        <v>1.89</v>
-      </c>
-      <c r="E23">
-        <v>1.968</v>
-      </c>
-      <c r="F23">
-        <v>1.9059999999999999</v>
-      </c>
-      <c r="G23">
-        <v>1.89</v>
-      </c>
-      <c r="H23">
-        <v>1.984</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>400000</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>160000000</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="2"/>
-        <v>1.9275999999999995</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.76868</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1000</v>
       </c>
       <c r="B24">
         <v>500</v>
       </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>250000</v>
+      </c>
       <c r="D24">
-        <v>2.39</v>
-      </c>
-      <c r="E24">
-        <v>2.5459999999999998</v>
-      </c>
-      <c r="F24">
-        <v>2.327</v>
-      </c>
-      <c r="G24">
-        <v>2.327</v>
-      </c>
-      <c r="H24">
-        <v>2.5310000000000001</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>500000</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="1"/>
-        <v>250000000</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="2"/>
-        <v>2.4241999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.8647499999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1000</v>
       </c>
       <c r="B25">
         <v>600</v>
       </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
       <c r="D25">
-        <v>3.03</v>
-      </c>
-      <c r="E25">
-        <v>2.859</v>
-      </c>
-      <c r="F25">
-        <v>2.883</v>
-      </c>
-      <c r="G25">
-        <v>2.8740000000000001</v>
-      </c>
-      <c r="H25">
-        <v>2.9369999999999998</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>600000</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="1"/>
-        <v>360000000</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="2"/>
-        <v>2.9165999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.3067399999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1000</v>
       </c>
       <c r="B26">
         <v>700</v>
       </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>490000</v>
+      </c>
       <c r="D26">
-        <v>3.218</v>
-      </c>
-      <c r="E26">
-        <v>3.2490000000000001</v>
-      </c>
-      <c r="F26">
-        <v>3.5150000000000001</v>
-      </c>
-      <c r="G26">
-        <v>3.234</v>
-      </c>
-      <c r="H26">
-        <v>3.4990000000000001</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>700000</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="1"/>
-        <v>490000000</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="2"/>
-        <v>3.343</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.8305800000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1000</v>
       </c>
       <c r="B27">
         <v>800</v>
       </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>640000</v>
+      </c>
       <c r="D27">
-        <v>3.9359999999999999</v>
-      </c>
-      <c r="E27">
-        <v>3.718</v>
-      </c>
-      <c r="F27">
-        <v>4.0460000000000003</v>
-      </c>
-      <c r="G27">
-        <v>3.9670000000000001</v>
-      </c>
-      <c r="H27">
-        <v>4.093</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>800000</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="1"/>
-        <v>640000000</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="2"/>
-        <v>3.9519999999999995</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.9265600000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1000</v>
       </c>
       <c r="B28">
         <v>900</v>
       </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>810000</v>
+      </c>
       <c r="D28">
-        <v>4.343</v>
-      </c>
-      <c r="E28">
-        <v>4.3739999999999997</v>
-      </c>
-      <c r="F28">
-        <v>4.3579999999999997</v>
-      </c>
-      <c r="G28">
-        <v>4.2649999999999997</v>
-      </c>
-      <c r="H28">
-        <v>4.6550000000000002</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>900000</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="1"/>
-        <v>810000000</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="2"/>
-        <v>4.399</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10.345230000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1000</v>
       </c>
       <c r="B29">
         <v>1000</v>
       </c>
-      <c r="D29">
-        <v>4.9210000000000003</v>
-      </c>
-      <c r="E29">
-        <v>5.17</v>
-      </c>
-      <c r="F29">
-        <v>5.093</v>
-      </c>
-      <c r="G29">
-        <v>4.9669999999999996</v>
-      </c>
-      <c r="H29">
-        <v>4.7809999999999997</v>
-      </c>
-      <c r="J29">
+      <c r="C29">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="1"/>
-        <v>1000000000</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="2"/>
-        <v>4.9863999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>12.7727</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1000</v>
       </c>
       <c r="B30">
         <v>1100</v>
       </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1210000</v>
+      </c>
       <c r="D30">
-        <v>5.4509999999999996</v>
-      </c>
-      <c r="E30">
-        <v>5.4829999999999997</v>
-      </c>
-      <c r="F30">
-        <v>5.1239999999999997</v>
-      </c>
-      <c r="G30">
-        <v>5.1859999999999999</v>
-      </c>
-      <c r="H30">
-        <v>5.4050000000000002</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="0"/>
-        <v>1100000</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="1"/>
-        <v>1210000000</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="2"/>
-        <v>5.3298000000000005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>15.828340000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1000</v>
       </c>
       <c r="B31">
         <v>1200</v>
       </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>1440000</v>
+      </c>
       <c r="D31">
-        <v>6.1</v>
-      </c>
-      <c r="E31">
-        <v>5.67</v>
-      </c>
-      <c r="F31">
-        <v>6.1239999999999997</v>
-      </c>
-      <c r="G31">
-        <v>5.9669999999999996</v>
-      </c>
-      <c r="H31">
-        <v>6.0289999999999999</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>1200000</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="1"/>
-        <v>1440000000</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="2"/>
-        <v>5.9779999999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18.397200000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1000</v>
       </c>
       <c r="B32">
         <v>1300</v>
       </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>1690000</v>
+      </c>
       <c r="D32">
-        <v>6.5460000000000003</v>
-      </c>
-      <c r="E32">
-        <v>6.53</v>
-      </c>
-      <c r="F32">
-        <v>6.5919999999999996</v>
-      </c>
-      <c r="G32">
-        <v>6.0140000000000002</v>
-      </c>
-      <c r="H32">
-        <v>6.3109999999999999</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="0"/>
-        <v>1300000</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="1"/>
-        <v>1690000000</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="2"/>
-        <v>6.3986000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>21.9024</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1000</v>
       </c>
       <c r="B33">
         <v>1400</v>
       </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>1960000</v>
+      </c>
       <c r="D33">
-        <v>6.952</v>
-      </c>
-      <c r="E33">
-        <v>7.2969999999999997</v>
-      </c>
-      <c r="F33">
-        <v>7.28</v>
-      </c>
-      <c r="G33">
-        <v>7.17</v>
-      </c>
-      <c r="H33">
-        <v>7.03</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="0"/>
-        <v>1400000</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="1"/>
-        <v>1960000000</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="2"/>
-        <v>7.1457999999999995</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>24.91104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1000</v>
       </c>
       <c r="B34">
         <v>1500</v>
       </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>2250000</v>
+      </c>
       <c r="D34">
-        <v>7.6029999999999998</v>
-      </c>
-      <c r="E34">
-        <v>7.8570000000000002</v>
-      </c>
-      <c r="F34">
-        <v>7.4050000000000002</v>
-      </c>
-      <c r="G34">
-        <v>7.2009999999999996</v>
-      </c>
-      <c r="H34">
-        <v>7.4359999999999999</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="0"/>
-        <v>1500000</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="1"/>
-        <v>2250000000</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="2"/>
-        <v>7.5004000000000008</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>27.966149999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1000</v>
       </c>
       <c r="B35">
         <v>1600</v>
       </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>2560000</v>
+      </c>
       <c r="D35">
-        <v>8.0289999999999999</v>
-      </c>
-      <c r="E35">
-        <v>7.8890000000000002</v>
-      </c>
-      <c r="F35">
-        <v>7.8570000000000002</v>
-      </c>
-      <c r="G35">
-        <v>7.4989999999999997</v>
-      </c>
-      <c r="H35">
-        <v>7.5129999999999999</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
-        <v>1600000</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="1"/>
-        <v>2560000000</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="2"/>
-        <v>7.7573999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>33.766719999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1000</v>
       </c>
       <c r="B36">
         <v>1700</v>
       </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>2890000</v>
+      </c>
       <c r="D36">
-        <v>8.577</v>
-      </c>
-      <c r="E36">
-        <v>8.3409999999999993</v>
-      </c>
-      <c r="F36">
-        <v>8.0139999999999993</v>
-      </c>
-      <c r="G36">
-        <v>7.9829999999999997</v>
-      </c>
-      <c r="H36">
-        <v>8.1539999999999999</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="0"/>
-        <v>1700000</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="1"/>
-        <v>2890000000</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="2"/>
-        <v>8.2138000000000009</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>38.538490000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1000</v>
       </c>
       <c r="B37">
         <v>1800</v>
       </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>3240000</v>
+      </c>
       <c r="D37">
-        <v>9.0449999999999999</v>
-      </c>
-      <c r="E37">
-        <v>8.4510000000000005</v>
-      </c>
-      <c r="F37">
-        <v>9.2330000000000005</v>
-      </c>
-      <c r="G37">
-        <v>8.3260000000000005</v>
-      </c>
-      <c r="H37">
-        <v>8.6229999999999993</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="0"/>
-        <v>1800000</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="1"/>
-        <v>3240000000</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="2"/>
-        <v>8.7356000000000016</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>41.8536</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1000</v>
       </c>
       <c r="B38">
         <v>1900</v>
       </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>3610000</v>
+      </c>
       <c r="D38">
-        <v>9.17</v>
-      </c>
-      <c r="E38">
-        <v>9.5760000000000005</v>
-      </c>
-      <c r="F38">
-        <v>9.3409999999999993</v>
-      </c>
-      <c r="G38">
-        <v>9.5449999999999999</v>
-      </c>
-      <c r="H38">
-        <v>9.4350000000000005</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="0"/>
-        <v>1900000</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="1"/>
-        <v>3610000000</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="2"/>
-        <v>9.4134000000000011</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45.10904</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1000</v>
       </c>
       <c r="B39">
         <v>2000</v>
       </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>4000000</v>
+      </c>
       <c r="D39">
-        <v>10.029</v>
-      </c>
-      <c r="E39">
-        <v>9.7319999999999993</v>
-      </c>
-      <c r="F39">
-        <v>9.9979999999999993</v>
-      </c>
-      <c r="G39">
-        <v>10.528</v>
-      </c>
-      <c r="H39">
-        <v>9.9510000000000005</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="0"/>
-        <v>2000000</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="1"/>
-        <v>4000000000</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="2"/>
-        <v>10.047599999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>53.365600000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1000</v>
       </c>
       <c r="B40">
         <v>3000</v>
       </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>9000000</v>
+      </c>
       <c r="D40">
-        <v>14.84</v>
-      </c>
-      <c r="E40">
-        <v>14.481</v>
-      </c>
-      <c r="F40">
-        <v>14.622</v>
-      </c>
-      <c r="G40">
-        <v>15.292999999999999</v>
-      </c>
-      <c r="H40">
-        <v>15.356</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="0"/>
-        <v>3000000</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="1"/>
-        <v>9000000000</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="2"/>
-        <v>14.9184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>121.41240000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1000</v>
       </c>
       <c r="B41">
         <v>4000</v>
       </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>16000000</v>
+      </c>
       <c r="D41">
-        <v>19.963999999999999</v>
-      </c>
-      <c r="E41">
-        <v>19.728999999999999</v>
-      </c>
-      <c r="F41">
-        <v>18.859000000000002</v>
-      </c>
-      <c r="G41">
-        <v>19.167999999999999</v>
-      </c>
-      <c r="H41">
-        <v>20.026</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="0"/>
-        <v>4000000</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="1"/>
-        <v>16000000000</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="2"/>
-        <v>19.549199999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>219.8108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1000</v>
       </c>
       <c r="B42">
         <v>5000</v>
       </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>25000000</v>
+      </c>
       <c r="D42">
-        <v>25.478999999999999</v>
-      </c>
-      <c r="E42">
-        <v>23.916</v>
-      </c>
-      <c r="F42">
-        <v>26.024999999999999</v>
-      </c>
-      <c r="G42">
-        <v>23.806999999999999</v>
-      </c>
-      <c r="H42">
-        <v>24.713000000000001</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="0"/>
-        <v>5000000</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="1"/>
-        <v>25000000000</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="2"/>
-        <v>24.788</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>317.99650000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1000</v>
       </c>
       <c r="B43">
         <v>6000</v>
       </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>36000000</v>
+      </c>
       <c r="D43">
-        <v>31.14</v>
-      </c>
-      <c r="E43">
-        <v>31.34</v>
-      </c>
-      <c r="F43">
-        <v>31.097999999999999</v>
-      </c>
-      <c r="G43">
-        <v>30.853999999999999</v>
-      </c>
-      <c r="H43">
-        <v>30.779</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="0"/>
-        <v>6000000</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="1"/>
-        <v>36000000000</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="2"/>
-        <v>31.042200000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>485.31779999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1000</v>
       </c>
       <c r="B44">
         <v>7000</v>
       </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>49000000</v>
+      </c>
       <c r="D44">
-        <v>34.942999999999998</v>
-      </c>
-      <c r="E44">
-        <v>33.991999999999997</v>
-      </c>
-      <c r="F44">
-        <v>34.195</v>
-      </c>
-      <c r="G44">
-        <v>34.506999999999998</v>
-      </c>
-      <c r="H44">
-        <v>35.148000000000003</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="0"/>
-        <v>7000000</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="1"/>
-        <v>49000000000</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="2"/>
-        <v>34.557000000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>624.43849999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1000</v>
       </c>
       <c r="B45">
         <v>8000</v>
       </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>64000000</v>
+      </c>
       <c r="D45">
-        <v>39.194000000000003</v>
-      </c>
-      <c r="E45">
-        <v>37.732999999999997</v>
-      </c>
-      <c r="F45">
-        <v>37.771999999999998</v>
-      </c>
-      <c r="G45">
-        <v>39.942999999999998</v>
-      </c>
-      <c r="H45">
-        <v>39.384999999999998</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="0"/>
-        <v>8000000</v>
-      </c>
-      <c r="K45">
-        <f t="shared" si="1"/>
-        <v>64000000000</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="2"/>
-        <v>38.805399999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>800.80799999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1000</v>
       </c>
       <c r="B46">
         <v>9000</v>
       </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>81000000</v>
+      </c>
       <c r="D46">
-        <v>44.186</v>
-      </c>
-      <c r="E46">
-        <v>44.356000000000002</v>
-      </c>
-      <c r="F46">
-        <v>46.23</v>
-      </c>
-      <c r="G46">
-        <v>43.884999999999998</v>
-      </c>
-      <c r="H46">
-        <v>48.082999999999998</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="0"/>
-        <v>9000000</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="1"/>
-        <v>81000000000</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="2"/>
-        <v>45.347999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1085.076</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1000</v>
       </c>
       <c r="B47">
         <v>10000</v>
       </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>100000000</v>
+      </c>
       <c r="D47">
-        <v>50.935000000000002</v>
-      </c>
-      <c r="E47">
-        <v>50.287999999999997</v>
-      </c>
-      <c r="F47">
-        <v>49.488</v>
-      </c>
-      <c r="G47">
-        <v>50.189</v>
-      </c>
-      <c r="H47">
-        <v>48.395000000000003</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="0"/>
-        <v>10000000</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="1"/>
-        <v>100000000000</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="2"/>
-        <v>49.859000000000002</v>
+        <v>1289.54</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>